<commit_message>
Update 1-13-2021: New Home Value Adjustments
</commit_message>
<xml_diff>
--- a/geomapper/BLS_Zillow_Geo.xlsx
+++ b/geomapper/BLS_Zillow_Geo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathano/Documents/misc/PythonProjects/SO_reportdata_updater/geomapper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2AC287-7235-154D-B475-2879F9BFF312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E8D6E9-549F-234F-BBBB-6836F365CEAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54440" yWindow="580" windowWidth="30000" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16620" yWindow="-21140" windowWidth="32340" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4683" uniqueCount="1103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4684" uniqueCount="1103">
   <si>
     <t>United States</t>
   </si>
@@ -3728,12 +3728,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:G950"/>
+  <dimension ref="A1:G951"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A868" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E884" sqref="E884"/>
+      <pane ySplit="1" topLeftCell="A526" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C539" sqref="C539"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3767,7 +3766,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>102001</v>
       </c>
@@ -3881,7 +3880,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D8" s="6">
         <v>10760</v>
       </c>
@@ -3915,7 +3914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D10" s="6">
         <v>12120</v>
       </c>
@@ -4089,7 +4088,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D19" s="6">
         <v>22840</v>
       </c>
@@ -4523,7 +4522,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D41" s="6">
         <v>26260</v>
       </c>
@@ -5997,7 +5996,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="115" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D115" s="6">
         <v>72850</v>
       </c>
@@ -6091,7 +6090,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="120" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D120" s="6">
         <v>78700</v>
       </c>
@@ -7045,7 +7044,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="168" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D168" s="6">
         <v>21640</v>
       </c>
@@ -7639,7 +7638,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="198" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D198" s="6">
         <v>16140</v>
       </c>
@@ -7753,7 +7752,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="204" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D204" s="6">
         <v>22700</v>
       </c>
@@ -7927,7 +7926,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="213" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D213" s="6">
         <v>37800</v>
       </c>
@@ -8361,7 +8360,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D235" s="6">
         <v>16460</v>
       </c>
@@ -10036,7 +10035,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="319" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D319" s="6">
         <v>16420</v>
       </c>
@@ -10550,7 +10549,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="345" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D345" s="6">
         <v>27660</v>
       </c>
@@ -10744,7 +10743,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="355" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D355" s="6">
         <v>70450</v>
       </c>
@@ -10818,7 +10817,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="359" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D359" s="6">
         <v>74500</v>
       </c>
@@ -10832,7 +10831,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="360" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D360" s="6">
         <v>75550</v>
       </c>
@@ -10846,7 +10845,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="361" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D361" s="6">
         <v>76150</v>
       </c>
@@ -11100,7 +11099,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="374" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D374" s="6">
         <v>72250</v>
       </c>
@@ -11154,7 +11153,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="377" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D377" s="6">
         <v>77950</v>
       </c>
@@ -11168,7 +11167,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="378" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D378" s="6">
         <v>78850</v>
       </c>
@@ -11962,7 +11961,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="418" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D418" s="6">
         <v>21860</v>
       </c>
@@ -12016,7 +12015,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="421" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D421" s="6">
         <v>24330</v>
       </c>
@@ -12610,7 +12609,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="451" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D451" s="6">
         <v>39500</v>
       </c>
@@ -13204,7 +13203,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="481" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D481" s="6">
         <v>48500</v>
       </c>
@@ -14318,7 +14317,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="537" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="537" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D537" s="6">
         <v>71500</v>
       </c>
@@ -14552,18 +14551,24 @@
         <v>507</v>
       </c>
     </row>
-    <row r="549" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A549" s="6">
+    <row r="549" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A549" s="5">
         <v>394383</v>
       </c>
-      <c r="B549" s="6" t="s">
+      <c r="B549" s="5" t="s">
         <v>522</v>
       </c>
-      <c r="C549" s="6" t="s">
+      <c r="C549" s="5" t="s">
         <v>517</v>
       </c>
-      <c r="G549" s="6" t="s">
-        <v>1033</v>
+      <c r="D549" s="5">
+        <v>13620</v>
+      </c>
+      <c r="E549" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="F549" s="5" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="550" spans="1:7" x14ac:dyDescent="0.2">
@@ -14606,7 +14611,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="552" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="552" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D552" s="6">
         <v>73050</v>
       </c>
@@ -14660,7 +14665,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="555" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="555" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D555" s="6">
         <v>74350</v>
       </c>
@@ -14694,7 +14699,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="557" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="557" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D557" s="6">
         <v>76900</v>
       </c>
@@ -14828,7 +14833,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="564" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D564" s="6">
         <v>16100</v>
       </c>
@@ -15082,7 +15087,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="577" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="577" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D577" s="6">
         <v>40760</v>
       </c>
@@ -18116,7 +18121,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="729" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="729" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D729" s="6">
         <v>41260</v>
       </c>
@@ -18790,7 +18795,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="763" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="763" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D763" s="6">
         <v>15140</v>
       </c>
@@ -19504,7 +19509,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="799" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="799" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D799" s="6">
         <v>14300</v>
       </c>
@@ -20278,7 +20283,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="838" spans="1:7" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="838" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D838" s="6">
         <v>37770</v>
       </c>
@@ -22532,12 +22537,12 @@
         <v>862</v>
       </c>
     </row>
+    <row r="951" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B951"/>
+      <c r="E951"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G950" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="6">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G950" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C876">
     <sortCondition ref="C1:C876"/>
     <sortCondition ref="B1:B876"/>

</xml_diff>